<commit_message>
minor update to check for deployment
</commit_message>
<xml_diff>
--- a/Processed_dataset_on_PlaqView.xlsx
+++ b/Processed_dataset_on_PlaqView.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive-115504944321605412484/My Drive/UVA/Grad School/Projects/PlaqView/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C516FD-02A4-2A4C-8D6D-3E3720E27F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB90EC6F-1D22-2A49-8BB2-DD19DABB455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="48120" windowHeight="24520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39260" windowHeight="24520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Journal</t>
   </si>
@@ -196,24 +196,6 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/1hpux30cN3BCTrOujTuP26xZ3kxxzAeMS?usp=sharing</t>
-  </si>
-  <si>
-    <t>Li et al.</t>
-  </si>
-  <si>
-    <t>https://www.ahajournals.org/doi/10.1161/CIRCULATIONAHA.120.046528</t>
-  </si>
-  <si>
-    <t>Ascneding Thoracic Aorta</t>
-  </si>
-  <si>
-    <t>Aneurysm (ATAA)</t>
-  </si>
-  <si>
-    <t>11 Patients</t>
-  </si>
-  <si>
-    <t>Li_2020</t>
   </si>
 </sst>
 </file>
@@ -620,7 +602,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1051,45 +1033,19 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2020</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="5">
-        <v>48128</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="8">
-        <v>44489</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
@@ -15942,13 +15898,11 @@
     <hyperlink ref="D9" r:id="rId11" xr:uid="{A34E3B8C-A4E6-F846-9797-465D7254FB50}"/>
     <hyperlink ref="M9" r:id="rId12" xr:uid="{A2AB59CB-97EA-2B46-BE98-489C303C3F33}"/>
     <hyperlink ref="D10" r:id="rId13" xr:uid="{612CCCDD-12EF-1840-9ECF-21530D6D916B}"/>
-    <hyperlink ref="D11" r:id="rId14" xr:uid="{384FE234-48D7-F34F-9044-B2662F05A373}"/>
-    <hyperlink ref="M11" r:id="rId15" xr:uid="{D495C4CD-3EBF-9543-A466-B387164FF457}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>